<commit_message>
#64 Tasks list and creation form in webapp (WIP)
</commit_message>
<xml_diff>
--- a/sormas-backend/tools/Tasks.xlsx
+++ b/sormas-backend/tools/Tasks.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
     <sheet name="Enum" sheetId="2" r:id="rId2"/>
+    <sheet name="Properties" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>Context</t>
   </si>
@@ -120,6 +121,54 @@
   </si>
   <si>
     <t>CODE</t>
+  </si>
+  <si>
+    <t>CAPTION</t>
+  </si>
+  <si>
+    <t>Caption</t>
+  </si>
+  <si>
+    <t>CASE_BURIAL</t>
+  </si>
+  <si>
+    <t>CASE_FINDING</t>
+  </si>
+  <si>
+    <t>CASE_INVESTIGATION</t>
+  </si>
+  <si>
+    <t>CASE_ISOLATION</t>
+  </si>
+  <si>
+    <t>CASE_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>CASE_TRANSPORT</t>
+  </si>
+  <si>
+    <t>PSYCHOLOGICAL_SUPPORT</t>
+  </si>
+  <si>
+    <t>PSYCHOSOCIAL_SUPPORT</t>
+  </si>
+  <si>
+    <t>CONTACT_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>CONTACT_TRACING</t>
+  </si>
+  <si>
+    <t>CONTACT_VISIT</t>
+  </si>
+  <si>
+    <t>INVESTIGATE_RUMOR</t>
+  </si>
+  <si>
+    <t>RUMOR_CREATOR</t>
+  </si>
+  <si>
+    <t>RUMOR_HANDLING</t>
   </si>
 </sst>
 </file>
@@ -539,18 +588,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="2" max="2" width="21.25" customWidth="1"/>
+    <col min="3" max="3" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,62 +608,70 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -622,36 +680,42 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -660,15 +724,18 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -677,15 +744,18 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -694,15 +764,18 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -711,15 +784,18 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -728,15 +804,18 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -745,15 +824,18 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -762,15 +844,18 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -779,15 +864,18 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -796,15 +884,18 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -813,15 +904,18 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -842,7 +936,7 @@
   <dimension ref="A1:D237"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C2" sqref="C2:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,7 +963,7 @@
         <v>CASE_BURIAL(TaskContext.CASE),</v>
       </c>
       <c r="C2" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B2)," ","_")</f>
+        <f>Tasks!B2</f>
         <v>CASE_BURIAL</v>
       </c>
       <c r="D2" t="str">
@@ -883,7 +977,7 @@
         <v>CASE_FINDING(TaskContext.CASE),</v>
       </c>
       <c r="C3" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B3)," ","_")</f>
+        <f>Tasks!B3</f>
         <v>CASE_FINDING</v>
       </c>
       <c r="D3" t="str">
@@ -897,7 +991,7 @@
         <v>CASE_INVESTIGATION(TaskContext.CASE),</v>
       </c>
       <c r="C4" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B4)," ","_")</f>
+        <f>Tasks!B4</f>
         <v>CASE_INVESTIGATION</v>
       </c>
       <c r="D4" t="str">
@@ -911,7 +1005,7 @@
         <v>CASE_ISOLATION(TaskContext.CASE),</v>
       </c>
       <c r="C5" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B5)," ","_")</f>
+        <f>Tasks!B5</f>
         <v>CASE_ISOLATION</v>
       </c>
       <c r="D5" t="str">
@@ -925,7 +1019,7 @@
         <v>CASE_MANAGEMENT(TaskContext.CASE),</v>
       </c>
       <c r="C6" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B6)," ","_")</f>
+        <f>Tasks!B6</f>
         <v>CASE_MANAGEMENT</v>
       </c>
       <c r="D6" t="str">
@@ -939,7 +1033,7 @@
         <v>CASE_TRANSPORT(TaskContext.CASE),</v>
       </c>
       <c r="C7" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B7)," ","_")</f>
+        <f>Tasks!B7</f>
         <v>CASE_TRANSPORT</v>
       </c>
       <c r="D7" t="str">
@@ -953,7 +1047,7 @@
         <v>PSYCHOLOGICAL_SUPPORT(TaskContext.CASE),</v>
       </c>
       <c r="C8" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B8)," ","_")</f>
+        <f>Tasks!B8</f>
         <v>PSYCHOLOGICAL_SUPPORT</v>
       </c>
       <c r="D8" t="str">
@@ -967,7 +1061,7 @@
         <v>PSYCHOSOCIAL_SUPPORT(TaskContext.CASE),</v>
       </c>
       <c r="C9" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B9)," ","_")</f>
+        <f>Tasks!B9</f>
         <v>PSYCHOSOCIAL_SUPPORT</v>
       </c>
       <c r="D9" t="str">
@@ -981,7 +1075,7 @@
         <v>CONTACT_MANAGEMENT(TaskContext.CONTACT),</v>
       </c>
       <c r="C10" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B10)," ","_")</f>
+        <f>Tasks!B10</f>
         <v>CONTACT_MANAGEMENT</v>
       </c>
       <c r="D10" t="str">
@@ -995,7 +1089,7 @@
         <v>CONTACT_TRACING(TaskContext.CONTACT),</v>
       </c>
       <c r="C11" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B11)," ","_")</f>
+        <f>Tasks!B11</f>
         <v>CONTACT_TRACING</v>
       </c>
       <c r="D11" t="str">
@@ -1009,7 +1103,7 @@
         <v>CONTACT_VISIT(TaskContext.CONTACT),</v>
       </c>
       <c r="C12" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B12)," ","_")</f>
+        <f>Tasks!B12</f>
         <v>CONTACT_VISIT</v>
       </c>
       <c r="D12" t="str">
@@ -1023,7 +1117,7 @@
         <v>INVESTIGATE_RUMOR(TaskContext.EVENT),</v>
       </c>
       <c r="C13" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B13)," ","_")</f>
+        <f>Tasks!B13</f>
         <v>INVESTIGATE_RUMOR</v>
       </c>
       <c r="D13" t="str">
@@ -1037,7 +1131,7 @@
         <v>RUMOR_CREATOR(TaskContext.EVENT),</v>
       </c>
       <c r="C14" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B14)," ","_")</f>
+        <f>Tasks!B14</f>
         <v>RUMOR_CREATOR</v>
       </c>
       <c r="D14" t="str">
@@ -1051,7 +1145,7 @@
         <v>RUMOR_HANDLING(TaskContext.EVENT),</v>
       </c>
       <c r="C15" t="str">
-        <f>SUBSTITUTE(UPPER(Tasks!B15)," ","_")</f>
+        <f>Tasks!B15</f>
         <v>RUMOR_HANDLING</v>
       </c>
       <c r="D15" t="str">
@@ -2573,6 +2667,442 @@
       <c r="C237" t="str">
         <f>SUBSTITUTE(UPPER(Tasks!B237)," ","_")</f>
         <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="23.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>"TaskType." &amp; C2 &amp; "=" &amp; D2</f>
+        <v>TaskType.CASE_BURIAL=case burial</v>
+      </c>
+      <c r="C2" t="str">
+        <f>Tasks!B2</f>
+        <v>CASE_BURIAL</v>
+      </c>
+      <c r="D2" t="str">
+        <f>Tasks!C2</f>
+        <v>case burial</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A30" si="0">"TaskType." &amp; C3 &amp; "=" &amp; D3</f>
+        <v>TaskType.CASE_FINDING=case finding</v>
+      </c>
+      <c r="C3" t="str">
+        <f>Tasks!B3</f>
+        <v>CASE_FINDING</v>
+      </c>
+      <c r="D3" t="str">
+        <f>Tasks!C3</f>
+        <v>case finding</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.CASE_INVESTIGATION=case investigation</v>
+      </c>
+      <c r="C4" t="str">
+        <f>Tasks!B4</f>
+        <v>CASE_INVESTIGATION</v>
+      </c>
+      <c r="D4" t="str">
+        <f>Tasks!C4</f>
+        <v>case investigation</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.CASE_ISOLATION=case isolation</v>
+      </c>
+      <c r="C5" t="str">
+        <f>Tasks!B5</f>
+        <v>CASE_ISOLATION</v>
+      </c>
+      <c r="D5" t="str">
+        <f>Tasks!C5</f>
+        <v>case isolation</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.CASE_MANAGEMENT=case management</v>
+      </c>
+      <c r="C6" t="str">
+        <f>Tasks!B6</f>
+        <v>CASE_MANAGEMENT</v>
+      </c>
+      <c r="D6" t="str">
+        <f>Tasks!C6</f>
+        <v>case management</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.CASE_TRANSPORT=case transport</v>
+      </c>
+      <c r="C7" t="str">
+        <f>Tasks!B7</f>
+        <v>CASE_TRANSPORT</v>
+      </c>
+      <c r="D7" t="str">
+        <f>Tasks!C7</f>
+        <v>case transport</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.PSYCHOLOGICAL_SUPPORT=psychological support</v>
+      </c>
+      <c r="C8" t="str">
+        <f>Tasks!B8</f>
+        <v>PSYCHOLOGICAL_SUPPORT</v>
+      </c>
+      <c r="D8" t="str">
+        <f>Tasks!C8</f>
+        <v>psychological support</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.PSYCHOSOCIAL_SUPPORT=psychosocial support</v>
+      </c>
+      <c r="C9" t="str">
+        <f>Tasks!B9</f>
+        <v>PSYCHOSOCIAL_SUPPORT</v>
+      </c>
+      <c r="D9" t="str">
+        <f>Tasks!C9</f>
+        <v>psychosocial support</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.CONTACT_MANAGEMENT=contact management</v>
+      </c>
+      <c r="C10" t="str">
+        <f>Tasks!B10</f>
+        <v>CONTACT_MANAGEMENT</v>
+      </c>
+      <c r="D10" t="str">
+        <f>Tasks!C10</f>
+        <v>contact management</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.CONTACT_TRACING=contact tracing</v>
+      </c>
+      <c r="C11" t="str">
+        <f>Tasks!B11</f>
+        <v>CONTACT_TRACING</v>
+      </c>
+      <c r="D11" t="str">
+        <f>Tasks!C11</f>
+        <v>contact tracing</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.CONTACT_VISIT=contact visit</v>
+      </c>
+      <c r="C12" t="str">
+        <f>Tasks!B12</f>
+        <v>CONTACT_VISIT</v>
+      </c>
+      <c r="D12" t="str">
+        <f>Tasks!C12</f>
+        <v>contact visit</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.INVESTIGATE_RUMOR=investigate rumor</v>
+      </c>
+      <c r="C13" t="str">
+        <f>Tasks!B13</f>
+        <v>INVESTIGATE_RUMOR</v>
+      </c>
+      <c r="D13" t="str">
+        <f>Tasks!C13</f>
+        <v>investigate rumor</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.RUMOR_CREATOR=rumor creator</v>
+      </c>
+      <c r="C14" t="str">
+        <f>Tasks!B14</f>
+        <v>RUMOR_CREATOR</v>
+      </c>
+      <c r="D14" t="str">
+        <f>Tasks!C14</f>
+        <v>rumor creator</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.RUMOR_HANDLING=rumor handling</v>
+      </c>
+      <c r="C15" t="str">
+        <f>Tasks!B15</f>
+        <v>RUMOR_HANDLING</v>
+      </c>
+      <c r="D15" t="str">
+        <f>Tasks!C15</f>
+        <v>rumor handling</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C16">
+        <f>Tasks!B16</f>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f>Tasks!C16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C17">
+        <f>Tasks!B17</f>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f>Tasks!C17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C18">
+        <f>Tasks!B18</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f>Tasks!C18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C19">
+        <f>Tasks!B19</f>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f>Tasks!C19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C20">
+        <f>Tasks!B20</f>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f>Tasks!C20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C21">
+        <f>Tasks!B21</f>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f>Tasks!C21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C22">
+        <f>Tasks!B22</f>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f>Tasks!C22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C23">
+        <f>Tasks!B23</f>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f>Tasks!C23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C24">
+        <f>Tasks!B24</f>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f>Tasks!C24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C25">
+        <f>Tasks!B25</f>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f>Tasks!C25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C26">
+        <f>Tasks!B26</f>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f>Tasks!C26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C27">
+        <f>Tasks!B27</f>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f>Tasks!C27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C28">
+        <f>Tasks!B28</f>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f>Tasks!C28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C29">
+        <f>Tasks!B29</f>
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <f>Tasks!C29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f t="shared" si="0"/>
+        <v>TaskType.0=0</v>
+      </c>
+      <c r="C30">
+        <f>Tasks!B30</f>
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f>Tasks!C30</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>